<commit_message>
Configured Data Driven Browser invocation in Abstract Test File
</commit_message>
<xml_diff>
--- a/src/main/java/resources/testData.xlsx
+++ b/src/main/java/resources/testData.xlsx
@@ -62,7 +62,7 @@
     <t>International Version</t>
   </si>
   <si>
-    <t>firefox</t>
+    <t>edge</t>
   </si>
 </sst>
 </file>
@@ -1253,7 +1253,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="5"/>

</xml_diff>